<commit_message>
Ya se pueden actualizar los catálogos
</commit_message>
<xml_diff>
--- a/v2/data/errores_al_cargar.xlsx
+++ b/v2/data/errores_al_cargar.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,9 +435,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="14" customWidth="1" min="1" max="1"/>
     <col width="14" customWidth="1" min="2" max="2"/>
-    <col width="49" customWidth="1" min="3" max="3"/>
+    <col width="33" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -460,7 +460,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>VDFUP001</t>
+          <t>GR3922</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -470,7 +470,186 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>POLVOS - FABRICACIONES DEL 04 AL 08 DE SEP.xlsx</t>
+          <t>produccion-lerma-semana-05.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>GR3890</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>sku invalido</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>produccion-lerma-semana-05.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ANSAGR4051</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>sku invalido</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>produccion-lerma-semana-05.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ANSAH340</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>sku invalido</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>produccion-lerma-semana-05.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>10481573</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>sku invalido</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>produccion-lerma-semana-05.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>GIFT81747334</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>sku invalido</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>produccion-lerma-semana-05.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>GIFT80863470</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>sku invalido</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>produccion-lerma-semana-05.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>11081214</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>sku invalido</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>produccion-lerma-semana-05.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>10595873</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>sku invalido</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>produccion-lerma-semana-05.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>GIFT79485824</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>sku invalido</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>produccion-lerma-semana-05.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10595875</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>sku invalido</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>produccion-lerma-semana-05.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>GIFT12659082</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>sku invalido</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>produccion-lerma-semana-05.xlsx</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Listo a la verga
</commit_message>
<xml_diff>
--- a/v2/data/errores_al_cargar.xlsx
+++ b/v2/data/errores_al_cargar.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,9 +435,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="10" customWidth="1" min="1" max="1"/>
     <col width="14" customWidth="1" min="2" max="2"/>
-    <col width="33" customWidth="1" min="3" max="3"/>
+    <col width="49" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -460,7 +460,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>GR3922</t>
+          <t>VDFUP001</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -470,186 +470,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>produccion-lerma-semana-05.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>GR3890</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>sku invalido</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>produccion-lerma-semana-05.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>ANSAGR4051</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>sku invalido</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>produccion-lerma-semana-05.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>ANSAH340</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>sku invalido</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>produccion-lerma-semana-05.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>10481573</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>sku invalido</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>produccion-lerma-semana-05.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>GIFT81747334</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>sku invalido</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>produccion-lerma-semana-05.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>GIFT80863470</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>sku invalido</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>produccion-lerma-semana-05.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>11081214</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>sku invalido</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>produccion-lerma-semana-05.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>10595873</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>sku invalido</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>produccion-lerma-semana-05.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>GIFT79485824</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>sku invalido</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>produccion-lerma-semana-05.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>10595875</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>sku invalido</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>produccion-lerma-semana-05.xlsx</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>GIFT12659082</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>sku invalido</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>produccion-lerma-semana-05.xlsx</t>
+          <t>POLVOS - FABRICACIONES DEL 04 AL 08 DE SEP.xlsx</t>
         </is>
       </c>
     </row>

</xml_diff>